<commit_message>
#73 Correction of the data in the physical model according to the changes made to the relational model due to feedback from SPRINT 1.
</commit_message>
<xml_diff>
--- a/plantFloorManager/SQL_Database/Dataset02_v2.xlsx
+++ b/plantFloorManager/SQL_Database/Dataset02_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://0cms6-my.sharepoint.com/personal/diogopereira_0cms6_onmicrosoft_com/Documents/Faculdade/Código 2º Ano/sem3-pi-2024-g094/plantFloorManager/SQL_Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="629" documentId="8_{61104BE5-191E-4C22-96ED-F0E59940F269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA2C3FEA-9700-4405-91DF-9A9D6EEA0195}"/>
+  <xr:revisionPtr revIDLastSave="676" documentId="8_{61104BE5-191E-4C22-96ED-F0E59940F269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79AA20D7-2953-46B8-880D-ABF8F5F2275D}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="1" activeTab="1" xr2:uid="{96054C54-0AC6-4E0E-AB4B-5CA509897BDA}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="2" activeTab="7" xr2:uid="{96054C54-0AC6-4E0E-AB4B-5CA509897BDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
@@ -1028,7 +1028,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="B9" sqref="B9:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1196,7 +1196,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B10" t="str">
-        <f t="shared" ref="B10:B17" si="0">_xlfn.CONCAT("insert into Customer(Customer_ID, NIF, Name, Address, Mobile_number, Email, type_ID, Country_ID, Status) values ('",A3,"', '",C3,"', '",B3,"', '",D3,", ",E3," ",F3,", ",G3,"', ",I3,", '",H3,"', 2, 620, 'Activated');")</f>
+        <f t="shared" ref="B10:B11" si="0">_xlfn.CONCAT("insert into Customer(Customer_ID, NIF, Name, Address, Mobile_number, Email, type_ID, Country_ID, Status) values ('",A3,"', '",C3,"', '",B3,"', '",D3,", ",E3," ",F3,", ",G3,"', ",I3,", '",H3,"', 2, 620, 'Activated');")</f>
         <v>insert into Customer(Customer_ID, NIF, Name, Address, Mobile_number, Email, type_ID, Country_ID, Status) values ('785', 'PT501245488', 'Tudo para a casa, Lda', 'R. Dr. Barros 93, 4465-219 São Mamede de Infesta, Portugal', 003518340500, 'me@neither.com', 2, 620, 'Activated');</v>
       </c>
     </row>
@@ -1253,8 +1253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D15D9EF7-7F05-4929-9267-83A028A1D45D}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1426,7 +1426,7 @@
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B23" t="str">
-        <f t="shared" ref="B23:B30" si="1">_xlfn.CONCAT("insert into BOM(Product_ID) values('",A3,"')",)</f>
+        <f t="shared" ref="B23:B28" si="1">_xlfn.CONCAT("insert into BOM(Product_ID) values('",A3,"')",)</f>
         <v>insert into BOM(Product_ID) values('AS12945S22')</v>
       </c>
     </row>
@@ -2974,10 +2974,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D833FD3A-319E-497B-BBC6-9FC6F2F78F3D}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69:B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2985,9 +2985,10 @@
     <col min="1" max="1" width="14.19921875" customWidth="1"/>
     <col min="2" max="2" width="17.73046875" customWidth="1"/>
     <col min="3" max="3" width="32.9296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="9.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>72</v>
       </c>
@@ -3001,7 +3002,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -3014,8 +3015,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -3028,8 +3032,11 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -3042,8 +3049,11 @@
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -3056,8 +3066,11 @@
       <c r="D5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -3070,8 +3083,11 @@
       <c r="D6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -3084,8 +3100,11 @@
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3098,8 +3117,11 @@
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -3112,8 +3134,11 @@
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -3126,8 +3151,11 @@
       <c r="D10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -3140,8 +3168,11 @@
       <c r="D11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -3154,8 +3185,11 @@
       <c r="D12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -3168,8 +3202,11 @@
       <c r="D13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -3182,8 +3219,11 @@
       <c r="D14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -3197,7 +3237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -3283,247 +3323,307 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B24" t="str">
-        <f>_xlfn.CONCAT("insert into Component(Component_ID, Component_Description) values ('",B2,"', '",C2,"');")</f>
-        <v>insert into Component(Component_ID, Component_Description) values ('PN12344A21', 'Screw M6 35 mm');</v>
+        <f>_xlfn.CONCAT("insert into Component(Component_ID, Component_Description, Part_ID) values (",F2,", '",C2,"', '",B2,"');")</f>
+        <v>insert into Component(Component_ID, Component_Description, Part_ID) values (1, 'Screw M6 35 mm', 'PN12344A21');</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B25" t="str">
-        <f t="shared" ref="B25:B43" si="0">_xlfn.CONCAT("insert into Component(Component_ID, Component_Description) values ('",B3,"', '",C3,"');")</f>
-        <v>insert into Component(Component_ID, Component_Description) values ('PN52384R50', '300x300 mm 5mm stainless steel sheet');</v>
+        <f t="shared" ref="B25:B33" si="0">_xlfn.CONCAT("insert into Component(Component_ID, Component_Description, Part_ID) values (",F3,", '",C3,"', '",B3,"');")</f>
+        <v>insert into Component(Component_ID, Component_Description, Part_ID) values (2, '300x300 mm 5mm stainless steel sheet', 'PN52384R50');</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B26" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Component(Component_ID, Component_Description) values ('PN52384R10', '300x300 mm 1mm stainless steel sheet');</v>
+        <v>insert into Component(Component_ID, Component_Description, Part_ID) values (3, '300x300 mm 1mm stainless steel sheet', 'PN52384R10');</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B27" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Component(Component_ID, Component_Description) values ('PN18544A21', 'Rivet 6 mm');</v>
+        <v>insert into Component(Component_ID, Component_Description, Part_ID) values (4, 'Rivet 6 mm', 'PN18544A21');</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B28" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Component(Component_ID, Component_Description) values ('PN18544C21', 'Stainless steel handle model U6');</v>
+        <v>insert into Component(Component_ID, Component_Description, Part_ID) values (5, 'Stainless steel handle model U6', 'PN18544C21');</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B29" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Component(Component_ID, Component_Description) values ('PN18324C54', 'Stainless steel handle model R12');</v>
+        <v>insert into Component(Component_ID, Component_Description, Part_ID) values (6, 'Stainless steel handle model R12', 'PN18324C54');</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B30" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Component(Component_ID, Component_Description) values ('PN12344A21', 'Screw M6 35 mm');</v>
+        <v>insert into Component(Component_ID, Component_Description, Part_ID) values (7, 'Screw M6 35 mm', 'PN12344A21');</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B31" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Component(Component_ID, Component_Description) values ('PN52384R50', '300x300 mm 5mm stainless steel sheet');</v>
+        <v>insert into Component(Component_ID, Component_Description, Part_ID) values (8, '300x300 mm 5mm stainless steel sheet', 'PN52384R50');</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B32" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Component(Component_ID, Component_Description) values ('PN52384R10', '300x300 mm 1mm stainless steel sheet');</v>
+        <v>insert into Component(Component_ID, Component_Description, Part_ID) values (9, '300x300 mm 1mm stainless steel sheet', 'PN52384R10');</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B33" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Component(Component_ID, Component_Description) values ('PN18544A21', 'Rivet 6 mm');</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B34" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Component(Component_ID, Component_Description) values ('PN18544C21', 'Stainless steel handle model U6');</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B35" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Component(Component_ID, Component_Description) values ('PN18324C51', 'Stainless steel handle model R11');</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B36" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Component(Component_ID, Component_Description) values ('PN12344A21', 'Screw M6 35 mm');</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B37" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Component(Component_ID, Component_Description) values ('PN52384R45', '250x250 mm 5mm stainless steel sheet');</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B38" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Component(Component_ID, Component_Description) values ('PN52384R12', '250x250 mm 1mm stainless steel sheet');</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B39" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Component(Component_ID, Component_Description) values ('PN18544A21', 'Rivet 6 mm');</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B40" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Component(Component_ID, Component_Description) values ('PN18544C21', 'Stainless steel handle model U6');</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B41" t="str">
-        <f>_xlfn.CONCAT("insert into Component(Component_ID, Component_Description) values ('",B19,"', '",C19,"');")</f>
-        <v>insert into Component(Component_ID, Component_Description) values ('PN18324C51', 'Stainless steel handle model R11');</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B42" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Component(Component_ID, Component_Description) values ('PN52384R45', '250x250 mm 5mm stainless steel sheet');</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B43" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into Component(Component_ID, Component_Description) values ('PN18324C91', 'Stainless steel handle model S26');</v>
+        <v>insert into Component(Component_ID, Component_Description, Part_ID) values (10, 'Rivet 6 mm', 'PN18544A21');</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B47" t="str">
-        <f>_xlfn.CONCAT("insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('",A2,"', '",B2,"', ",D2,");")</f>
-        <v>insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('AS12945S22', 'PN12344A21', 1);</v>
+        <f>_xlfn.CONCAT("insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('",B2,"', '",A2,"', ",D2,");")</f>
+        <v>insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('PN12344A21', 'AS12945S22', 1);</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B48" t="str">
-        <f t="shared" ref="B48:B66" si="1">_xlfn.CONCAT("insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('",A3,"', '",B3,"', ",D3,");")</f>
-        <v>insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('AS12945S22', 'PN52384R50', 1);</v>
+        <f t="shared" ref="B48:B71" si="1">_xlfn.CONCAT("insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('",B3,"', '",A3,"', ",D3,");")</f>
+        <v>insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('PN52384R50', 'AS12945S22', 1);</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B49" t="str">
         <f t="shared" si="1"/>
-        <v>insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('AS12945S22', 'PN52384R10', 1);</v>
+        <v>insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('PN52384R10', 'AS12945S22', 1);</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B50" t="str">
         <f t="shared" si="1"/>
-        <v>insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('AS12945S22', 'PN18544A21', 4);</v>
+        <v>insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('PN18544A21', 'AS12945S22', 4);</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B51" t="str">
         <f t="shared" si="1"/>
-        <v>insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('AS12945S22', 'PN18544C21', 2);</v>
+        <v>insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('PN18544C21', 'AS12945S22', 2);</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B52" t="str">
         <f t="shared" si="1"/>
-        <v>insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('AS12945S22', 'PN18324C54', 1);</v>
+        <v>insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('PN18324C54', 'AS12945S22', 1);</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B53" t="str">
         <f t="shared" si="1"/>
-        <v>insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('AS12945S20', 'PN12344A21', 1);</v>
+        <v>insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('PN12344A21', 'AS12945S20', 1);</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B54" t="str">
         <f t="shared" si="1"/>
-        <v>insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('AS12945S20', 'PN52384R50', 1);</v>
+        <v>insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('PN52384R50', 'AS12945S20', 1);</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B55" t="str">
         <f t="shared" si="1"/>
-        <v>insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('AS12945S20', 'PN52384R10', 1);</v>
+        <v>insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('PN52384R10', 'AS12945S20', 1);</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B56" t="str">
         <f t="shared" si="1"/>
-        <v>insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('AS12945S20', 'PN18544A21', 4);</v>
+        <v>insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('PN18544A21', 'AS12945S20', 4);</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B57" t="str">
         <f t="shared" si="1"/>
-        <v>insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('AS12945S20', 'PN18544C21', 2);</v>
+        <v>insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('PN18544C21', 'AS12945S20', 2);</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B58" t="str">
         <f t="shared" si="1"/>
-        <v>insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('AS12945S20', 'PN18324C51', 1);</v>
+        <v>insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('PN18324C51', 'AS12945S20', 1);</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B59" t="str">
         <f t="shared" si="1"/>
-        <v>insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('AS12945S17', 'PN12344A21', 1);</v>
+        <v>insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('PN12344A21', 'AS12945S17', 1);</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B60" t="str">
         <f t="shared" si="1"/>
-        <v>insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('AS12945S17', 'PN52384R45', 1);</v>
+        <v>insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('PN52384R45', 'AS12945S17', 1);</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B61" t="str">
         <f t="shared" si="1"/>
-        <v>insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('AS12945S17', 'PN52384R12', 1);</v>
+        <v>insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('PN52384R12', 'AS12945S17', 1);</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B62" t="str">
         <f t="shared" si="1"/>
-        <v>insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('AS12945S17', 'PN18544A21', 4);</v>
+        <v>insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('PN18544A21', 'AS12945S17', 4);</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B63" t="str">
         <f t="shared" si="1"/>
-        <v>insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('AS12945S17', 'PN18544C21', 2);</v>
+        <v>insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('PN18544C21', 'AS12945S17', 2);</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B64" t="str">
-        <f>_xlfn.CONCAT("insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('",A19,"', '",B19,"', ",D19,");")</f>
-        <v>insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('AS12945S17', 'PN18324C51', 1);</v>
+        <f t="shared" si="1"/>
+        <v>insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('PN18324C51', 'AS12945S17', 1);</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B65" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('AS12945P17', 'PN52384R45', 1);</v>
+        <f>_xlfn.CONCAT("insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('",B20,"', '",A20,"', ",D20,");")</f>
+        <v>insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('PN52384R45', 'AS12945P17', 1);</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B66" t="str">
         <f t="shared" si="1"/>
-        <v>insert into BOM(Product_ID, Component_ID, Component_Quantity) values ('AS12945P17', 'PN18324C91', 1);</v>
+        <v>insert into BOM_Part(Part_ID, Product_ID, Part_Quantity) values ('PN18324C91', 'AS12945P17', 1);</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B69" t="str">
+        <f>_xlfn.CONCAT("insert into Part(Part_ID) values ('",B2,"');")</f>
+        <v>insert into Part(Part_ID) values ('PN12344A21');</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B70" t="str">
+        <f>_xlfn.CONCAT("insert into Part(Part_ID) values ('",B3,"');")</f>
+        <v>insert into Part(Part_ID) values ('PN52384R50');</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B71" t="str">
+        <f>_xlfn.CONCAT("insert into Part(Part_ID) values ('",B4,"');")</f>
+        <v>insert into Part(Part_ID) values ('PN52384R10');</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B72" t="str">
+        <f>_xlfn.CONCAT("insert into Part(Part_ID) values ('",B5,"');")</f>
+        <v>insert into Part(Part_ID) values ('PN18544A21');</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B73" t="str">
+        <f>_xlfn.CONCAT("insert into Part(Part_ID) values ('",B6,"');")</f>
+        <v>insert into Part(Part_ID) values ('PN18544C21');</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B74" t="str">
+        <f>_xlfn.CONCAT("insert into Part(Part_ID) values ('",B7,"');")</f>
+        <v>insert into Part(Part_ID) values ('PN18324C54');</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B75" t="str">
+        <f>_xlfn.CONCAT("insert into Part(Part_ID) values ('",B8,"');")</f>
+        <v>insert into Part(Part_ID) values ('PN12344A21');</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B76" t="str">
+        <f>_xlfn.CONCAT("insert into Part(Part_ID) values ('",B9,"');")</f>
+        <v>insert into Part(Part_ID) values ('PN52384R50');</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B77" t="str">
+        <f>_xlfn.CONCAT("insert into Part(Part_ID) values ('",B10,"');")</f>
+        <v>insert into Part(Part_ID) values ('PN52384R10');</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B78" t="str">
+        <f>_xlfn.CONCAT("insert into Part(Part_ID) values ('",B11,"');")</f>
+        <v>insert into Part(Part_ID) values ('PN18544A21');</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B79" t="str">
+        <f>_xlfn.CONCAT("insert into Part(Part_ID) values ('",B12,"');")</f>
+        <v>insert into Part(Part_ID) values ('PN18544C21');</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B80" t="str">
+        <f>_xlfn.CONCAT("insert into Part(Part_ID) values ('",B13,"');")</f>
+        <v>insert into Part(Part_ID) values ('PN18324C51');</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B81" t="str">
+        <f>_xlfn.CONCAT("insert into Part(Part_ID) values ('",B14,"');")</f>
+        <v>insert into Part(Part_ID) values ('PN12344A21');</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B82" t="str">
+        <f>_xlfn.CONCAT("insert into Part(Part_ID) values ('",B15,"');")</f>
+        <v>insert into Part(Part_ID) values ('PN52384R45');</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B83" t="str">
+        <f>_xlfn.CONCAT("insert into Part(Part_ID) values ('",B16,"');")</f>
+        <v>insert into Part(Part_ID) values ('PN52384R12');</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B84" t="str">
+        <f>_xlfn.CONCAT("insert into Part(Part_ID) values ('",B17,"');")</f>
+        <v>insert into Part(Part_ID) values ('PN18544A21');</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B85" t="str">
+        <f>_xlfn.CONCAT("insert into Part(Part_ID) values ('",B18,"');")</f>
+        <v>insert into Part(Part_ID) values ('PN18544C21');</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B86" t="str">
+        <f>_xlfn.CONCAT("insert into Part(Part_ID) values ('",B19,"');")</f>
+        <v>insert into Part(Part_ID) values ('PN18324C51');</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B87" t="str">
+        <f>_xlfn.CONCAT("insert into Part(Part_ID) values ('",B20,"');")</f>
+        <v>insert into Part(Part_ID) values ('PN52384R45');</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B88" t="str">
+        <f>_xlfn.CONCAT("insert into Part(Part_ID) values ('",B21,"');")</f>
+        <v>insert into Part(Part_ID) values ('PN18324C91');</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3564,8 +3664,8 @@
         <v>1</v>
       </c>
       <c r="E2" t="str">
-        <f>_xlfn.CONCAT("insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values ('",A2,"', ",B2,", ",C2,");")</f>
-        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values ('125', 5647, 1);</v>
+        <f>_xlfn.CONCAT("insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values (",A2,", ",B2,", ",C2,");")</f>
+        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values (125, 5647, 1);</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
@@ -3579,8 +3679,8 @@
         <v>2</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E18" si="0">_xlfn.CONCAT("insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values ('",A3,"', ",B3,", ",C3,");")</f>
-        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values ('125', 5647, 2);</v>
+        <f t="shared" ref="E3:E17" si="0">_xlfn.CONCAT("insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values (",A3,", ",B3,", ",C3,");")</f>
+        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values (125, 5647, 2);</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
@@ -3595,7 +3695,7 @@
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values ('125', 5649, 3);</v>
+        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values (125, 5649, 3);</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -3610,7 +3710,7 @@
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values ('125', 5651, 4);</v>
+        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values (125, 5651, 4);</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
@@ -3625,7 +3725,7 @@
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values ('125', 5653, 5);</v>
+        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values (125, 5653, 5);</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -3640,7 +3740,7 @@
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values ('125', 5659, 6);</v>
+        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values (125, 5659, 6);</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
@@ -3655,7 +3755,7 @@
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values ('125', 5669, 7);</v>
+        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values (125, 5669, 7);</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
@@ -3670,7 +3770,7 @@
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values ('125', 5655, 8);</v>
+        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values (125, 5655, 8);</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
@@ -3685,7 +3785,7 @@
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values ('125', 5657, 9);</v>
+        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values (125, 5657, 9);</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
@@ -3700,7 +3800,7 @@
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
-        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values ('125', 5661, 10);</v>
+        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values (125, 5661, 10);</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
@@ -3715,7 +3815,7 @@
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
-        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values ('125', 5667, 11);</v>
+        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values (125, 5667, 11);</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
@@ -3730,7 +3830,7 @@
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
-        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values ('125', 5663, 12);</v>
+        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values (125, 5663, 12);</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
@@ -3745,7 +3845,7 @@
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
-        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values ('132', 5681, 1);</v>
+        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values (132, 5681, 1);</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
@@ -3760,7 +3860,7 @@
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
-        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values ('132', 5682, 2);</v>
+        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values (132, 5682, 2);</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
@@ -3775,7 +3875,7 @@
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
-        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values ('132', 5683, 3);</v>
+        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values (132, 5683, 3);</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
@@ -3790,7 +3890,7 @@
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
-        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values ('132', 5665, 4);</v>
+        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values (132, 5665, 4);</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
@@ -3804,12 +3904,12 @@
         <v>5</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values ('132', 5688, 5);</v>
+        <f>_xlfn.CONCAT("insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values (",A18,", ",B18,", ",C18,");")</f>
+        <v>insert into BOO(Product_Family_ID, Manufacturing_Operation_ID, Operation_Order) values (132, 5688, 5);</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>